<commit_message>
reknitted to fix issues
</commit_message>
<xml_diff>
--- a/Manuscript/lab_citations.xlsx
+++ b/Manuscript/lab_citations.xlsx
@@ -10811,8 +10811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7D04037-31D1-FA46-9B1F-17F7D6889BBD}">
   <dimension ref="A1:F906"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A869" zoomScale="198" zoomScaleNormal="198" workbookViewId="0">
-      <selection activeCell="C890" sqref="C890"/>
+    <sheetView tabSelected="1" topLeftCell="A877" zoomScale="198" zoomScaleNormal="198" workbookViewId="0">
+      <selection activeCell="C882" sqref="C882"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>